<commit_message>
Reimbursement Requests Submitted 5/23/13. update
</commit_message>
<xml_diff>
--- a/Budgets/2012 - 2013/Robotics Club Budget.xlsx
+++ b/Budgets/2012 - 2013/Robotics Club Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="19440" windowHeight="14310" tabRatio="693"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="19440" windowHeight="14310" tabRatio="693" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -235,9 +235,6 @@
     <t>Josh Crook</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Panels</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>SGA: 1500, NTMA:?</t>
+  </si>
+  <si>
+    <t>Thrusters</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -823,16 +823,16 @@
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M2">
         <v>9000</v>
       </c>
       <c r="N2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,16 +857,16 @@
         <v>10000</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="29">
         <f>('Incoming Funds'!G3)-(D6+D7+D9+D14+D18+D22)</f>
-        <v>23101.53</v>
+        <v>21879.25</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4">
         <v>5400</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J5" s="6">
         <v>2000</v>
@@ -919,7 +919,7 @@
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J6" s="6">
         <v>1000</v>
@@ -951,7 +951,7 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J7" s="6">
         <v>2000</v>
@@ -983,7 +983,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="6">
         <v>400</v>
@@ -1008,22 +1008,22 @@
       </c>
       <c r="D9" s="21">
         <f>B9-F9</f>
-        <v>1225.5900000000001</v>
+        <v>1182.8699999999999</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="20">
         <f>'IGVC Software'!H3</f>
-        <v>774.40999999999985</v>
+        <v>817.13000000000011</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9">
         <v>500</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J10">
         <v>1500</v>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J12" s="6">
         <v>0</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -1146,13 +1146,13 @@
       <c r="G13" s="9"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J13" s="6">
         <v>1000</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -1174,22 +1174,22 @@
       </c>
       <c r="D14" s="21">
         <f>B14-F14</f>
-        <v>1887.2099999999982</v>
+        <v>3152.2099999999982</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="20">
         <f>MATE!H3</f>
-        <v>3112.7900000000018</v>
+        <v>1847.7900000000018</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J14" s="6">
         <v>500</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J15" s="6">
         <v>1450</v>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J20" s="6">
         <f>SUM(J3:J15)</f>
@@ -1497,11 +1497,11 @@
       </c>
       <c r="D28" s="20">
         <f>SUM(D6,D7,D9,D10,D11,D12,D14,D15,D16,D18,D19,D20,D22:D26)</f>
-        <v>4610.909999999998</v>
+        <v>5833.1899999999978</v>
       </c>
       <c r="F28" s="20">
         <f>SUM(F6,F9:F10,F12,F14,F16,F18:F20,F22:F26)</f>
-        <v>12389.090000000002</v>
+        <v>11166.810000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1583,8 +1583,8 @@
   </sheetPr>
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,9 +1743,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>66</v>
       </c>
@@ -1771,12 +1771,9 @@
       <c r="E12">
         <v>415</v>
       </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -1791,7 +1788,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>69</v>
       </c>
@@ -1806,9 +1803,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>49</v>
@@ -1821,9 +1818,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="6"/>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>49</v>
@@ -1836,9 +1833,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="6"/>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>49</v>
@@ -1860,10 +1857,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1903,7 @@
       </c>
       <c r="H3" s="20">
         <f>2*E3-SUM(E:E)</f>
-        <v>774.40999999999985</v>
+        <v>817.13000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1914,7 +1911,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2">
         <v>41302</v>
@@ -1924,7 +1921,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>67</v>
       </c>
@@ -1935,13 +1932,13 @@
         <v>41413</v>
       </c>
       <c r="E5">
-        <v>183.72</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
@@ -1950,16 +1947,13 @@
         <v>41413</v>
       </c>
       <c r="E6">
-        <v>600</v>
-      </c>
-      <c r="F6" t="s">
-        <v>71</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -1970,6 +1964,12 @@
       <c r="E7">
         <v>425.92</v>
       </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1984,7 +1984,7 @@
   <dimension ref="A2:I36"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="H3" s="20">
         <f>2*E3-SUM(E:E)</f>
-        <v>3112.7900000000018</v>
+        <v>1847.7900000000018</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -2091,7 +2091,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
@@ -2270,6 +2270,18 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2">
+        <v>41414</v>
+      </c>
+      <c r="E20">
+        <v>1265</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>

</xml_diff>